<commit_message>
Deploying to master from  @ e173869b72fe567e0ea7fdf8bdf876106242f6b8 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_6-2-2.xlsx
+++ b/assets/excel/2022_6-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2C8686-BB0E-4D2A-8695-BBA6D212F225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83ED14CE-B914-45AD-AF28-1FD958F01048}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{6D20BA34-5F99-4BCC-BC15-D54A156181FF}"/>
   </bookViews>
@@ -396,7 +396,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +456,11 @@
       <sz val="6"/>
       <color theme="10"/>
       <name val="NDSFrutiger 45 Light"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="NDSFrutiger 55 Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -615,7 +620,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -739,6 +744,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1279,9 +1287,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:O384"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1721,7 +1727,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="23">
         <v>1</v>
       </c>
@@ -1731,22 +1737,22 @@
       <c r="D22" s="24">
         <v>2020</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="24">
         <v>90</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="24">
         <v>71</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="24">
         <v>26</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="24">
         <v>527</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="24">
         <v>259</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="24">
         <v>187</v>
       </c>
     </row>
@@ -2011,7 +2017,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="23">
         <v>2</v>
       </c>
@@ -2021,22 +2027,22 @@
       <c r="D32" s="24">
         <v>2020</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="24">
         <v>110</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="24">
         <v>76</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="24">
         <v>31</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="24">
         <v>608</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="24">
         <v>321</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="24">
         <v>292</v>
       </c>
     </row>
@@ -2359,7 +2365,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="23">
         <v>3</v>
       </c>
@@ -2369,22 +2375,22 @@
       <c r="D44" s="24">
         <v>2020</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="24">
         <v>75</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="24">
         <v>59</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="24">
         <v>24</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="24">
         <v>494</v>
       </c>
-      <c r="I44" s="22">
+      <c r="I44" s="24">
         <v>258</v>
       </c>
-      <c r="J44" s="22">
+      <c r="J44" s="24">
         <v>200</v>
       </c>
     </row>
@@ -2881,7 +2887,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="23">
         <v>4</v>
       </c>
@@ -2891,26 +2897,26 @@
       <c r="D62" s="24">
         <v>2020</v>
       </c>
-      <c r="E62" s="22">
+      <c r="E62" s="24">
         <v>74</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F62" s="24">
         <v>62</v>
       </c>
-      <c r="G62" s="22">
+      <c r="G62" s="24">
         <v>27</v>
       </c>
-      <c r="H62" s="22">
+      <c r="H62" s="24">
         <v>407</v>
       </c>
-      <c r="I62" s="22">
+      <c r="I62" s="24">
         <v>211</v>
       </c>
-      <c r="J62" s="22">
+      <c r="J62" s="24">
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="23">
         <v>0</v>
       </c>
@@ -2920,22 +2926,22 @@
       <c r="D63" s="24">
         <v>2020</v>
       </c>
-      <c r="E63" s="22">
+      <c r="E63" s="24">
         <v>87</v>
       </c>
-      <c r="F63" s="22">
+      <c r="F63" s="24">
         <v>67</v>
       </c>
-      <c r="G63" s="22">
+      <c r="G63" s="24">
         <v>27</v>
       </c>
-      <c r="H63" s="22">
+      <c r="H63" s="24">
         <v>504</v>
       </c>
-      <c r="I63" s="22">
+      <c r="I63" s="24">
         <v>263</v>
       </c>
-      <c r="J63" s="22">
+      <c r="J63" s="24">
         <v>233</v>
       </c>
     </row>
@@ -12150,5 +12156,6 @@
     <hyperlink ref="C384" r:id="rId1" xr:uid="{B77B2D50-DED9-4324-9352-4F7A2E82FE72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>